<commit_message>
Integrating Lana's Figure 1 and Figure 2 and fixing a bug with SIR plots for all DBs across all AESIs
</commit_message>
<xml_diff>
--- a/extras/CovidAesiReporting/extras/Censorship Worksheet.xlsx
+++ b/extras/CovidAesiReporting/extras/Censorship Worksheet.xlsx
@@ -59,7 +59,7 @@
     <author>tc={BE9E5AD4-BD47-47F5-A0F0-1858BA6BBD16}</author>
   </authors>
   <commentList>
-    <comment ref="Q25" authorId="0" shapeId="0">
+    <comment ref="Q24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="1" shapeId="0">
+    <comment ref="B25" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W26" authorId="2" shapeId="0">
+    <comment ref="W25" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="3" shapeId="0">
+    <comment ref="B27" authorId="3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H28" authorId="4" shapeId="0">
+    <comment ref="H27" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I28" authorId="5" shapeId="0">
+    <comment ref="I27" authorId="5" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J28" authorId="6" shapeId="0">
+    <comment ref="J27" authorId="6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -181,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K28" authorId="7" shapeId="0">
+    <comment ref="K27" authorId="7" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M28" authorId="8" shapeId="0">
+    <comment ref="M27" authorId="8" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N28" authorId="9" shapeId="0">
+    <comment ref="N27" authorId="9" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q28" authorId="10" shapeId="0">
+    <comment ref="Q27" authorId="10" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R28" authorId="11" shapeId="0">
+    <comment ref="R27" authorId="11" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S28" authorId="12" shapeId="0">
+    <comment ref="S27" authorId="12" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -289,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V28" authorId="13" shapeId="0">
+    <comment ref="V27" authorId="13" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -308,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W28" authorId="14" shapeId="0">
+    <comment ref="W27" authorId="14" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="132">
   <si>
     <t>Censorship Key</t>
   </si>
@@ -561,9 +561,6 @@
   </si>
   <si>
     <t>CPRD_AURUM</t>
-  </si>
-  <si>
-    <t>ULSM</t>
   </si>
   <si>
     <t>APHM</t>
@@ -873,7 +870,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -913,21 +910,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -954,7 +936,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1013,38 +995,36 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1115,7 +1095,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId2"/>
+              <asvg:svgBlip xmlns="" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1635,11 +1615,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W31"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,32 +1631,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -1886,8 +1866,8 @@
       <c r="M5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="26"/>
-      <c r="O5" s="24" t="s">
+      <c r="N5" s="25"/>
+      <c r="O5" s="23" t="s">
         <v>4</v>
       </c>
       <c r="P5" s="6" t="s">
@@ -1953,8 +1933,8 @@
       <c r="M6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="26"/>
-      <c r="O6" s="24" t="s">
+      <c r="N6" s="25"/>
+      <c r="O6" s="23" t="s">
         <v>4</v>
       </c>
       <c r="P6" s="6" t="s">
@@ -2154,8 +2134,8 @@
       <c r="M9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N9" s="26"/>
-      <c r="O9" s="24" t="s">
+      <c r="N9" s="25"/>
+      <c r="O9" s="23" t="s">
         <v>4</v>
       </c>
       <c r="P9" s="6" t="s">
@@ -2288,8 +2268,8 @@
       <c r="M11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="26"/>
-      <c r="O11" s="24" t="s">
+      <c r="N11" s="25"/>
+      <c r="O11" s="23" t="s">
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
@@ -2455,66 +2435,66 @@
       <c r="A14" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="23" t="s">
+      <c r="C14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="K14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L14" s="23" t="s">
+      <c r="K14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="M14" s="23" t="s">
+      <c r="M14" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="N14" s="26"/>
-      <c r="O14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="P14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="23" t="s">
+      <c r="N14" s="25"/>
+      <c r="O14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="R14" s="23" t="s">
+      <c r="R14" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="S14" s="23" t="s">
+      <c r="S14" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="T14" s="23" t="s">
+      <c r="T14" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="U14" s="23" t="s">
+      <c r="U14" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="V14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W14" s="24" t="s">
+      <c r="V14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W14" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2522,1102 +2502,1075 @@
       <c r="A15" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O15" s="26"/>
-      <c r="P15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V15" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W15" s="24" t="s">
+      <c r="B15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O15" s="25"/>
+      <c r="P15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W15" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="23" t="s">
+      <c r="B16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O16" s="26"/>
-      <c r="P16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V16" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W16" s="24" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O16" s="25"/>
+      <c r="P16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W16" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="23" t="s">
+      <c r="B17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="J17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O17" s="26"/>
-      <c r="P17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="23" t="s">
+      <c r="J17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="25"/>
+      <c r="P17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="R17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S17" s="23" t="s">
+      <c r="R17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S17" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="T17" s="23" t="s">
+      <c r="T17" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="U17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V17" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W17" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="U17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W17" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="22"/>
-    </row>
-    <row r="19" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="B18" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="24"/>
+      <c r="G18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O18" s="25"/>
+      <c r="P18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W18" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="G19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O19" s="25"/>
+      <c r="P19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W19" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="24"/>
+      <c r="G20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" s="25"/>
+      <c r="P20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R20" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="S20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W20" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O19" s="26"/>
-      <c r="P19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V19" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W19" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N20" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="O20" s="26"/>
-      <c r="P20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V20" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W20" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O21" s="26"/>
-      <c r="P21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="24" t="s">
+      <c r="C21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="25"/>
+      <c r="P21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="23" t="s">
         <v>4</v>
       </c>
       <c r="R21" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="S21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W21" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="S21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W21" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O22" s="26"/>
-      <c r="P22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V22" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W22" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+      <c r="C22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="24"/>
+      <c r="G22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" s="25"/>
+      <c r="P22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W22" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>82</v>
       </c>
       <c r="B23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="24"/>
+      <c r="G23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="25"/>
+      <c r="O23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W23" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="24"/>
+      <c r="G24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O24" s="25"/>
+      <c r="P24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W24" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O25" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="P25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="R25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="S25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="T25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="U25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="V25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="W25" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O23" s="26"/>
-      <c r="P23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V23" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W23" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N24" s="26"/>
-      <c r="O24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="P24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V24" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W24" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O25" s="26"/>
-      <c r="P25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V25" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W25" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="M26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="N26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="O26" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="P26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="R26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="S26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="T26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="U26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="V26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="W26" s="33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="24"/>
+      <c r="G26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N26" s="25"/>
+      <c r="O26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W26" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>87</v>
       </c>
       <c r="B27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="24"/>
+      <c r="G27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N27" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="O27" s="25"/>
+      <c r="P27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V27" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="W27" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N27" s="26"/>
-      <c r="O27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="P27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V27" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W27" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N28" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="O28" s="26"/>
-      <c r="P28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U28" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V28" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="W28" s="24" t="s">
+      <c r="C28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="24"/>
+      <c r="G28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O28" s="25"/>
+      <c r="P28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W28" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>89</v>
       </c>
       <c r="B29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="24"/>
+      <c r="G29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O29" s="25"/>
+      <c r="P29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W29" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="25"/>
-      <c r="G29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O29" s="26"/>
-      <c r="P29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V29" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W29" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" s="24" t="s">
+      <c r="C30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="24"/>
+      <c r="G30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="23" t="s">
         <v>4</v>
       </c>
       <c r="J30" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="K30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O30" s="26"/>
-      <c r="P30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W30" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M31" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M30" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="N31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O31" s="26"/>
-      <c r="P31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="R31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="U31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="V31" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W31" s="24" t="s">
+      <c r="N30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O30" s="25"/>
+      <c r="P30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="S30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="V30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="W30" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3647,10 +3600,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="19" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="43"/>
+      <c r="A1" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3662,10 +3615,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
         <v>93</v>
-      </c>
-      <c r="B3" t="s">
-        <v>94</v>
       </c>
       <c r="C3">
         <v>71</v>
@@ -3688,10 +3641,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
         <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>96</v>
       </c>
       <c r="C4">
         <v>21</v>
@@ -3744,10 +3697,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5">
         <v>71</v>
@@ -3797,354 +3750,354 @@
   <sheetData>
     <row r="1" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="H1" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="I1" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="J1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="19" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" t="s">
         <v>108</v>
       </c>
-      <c r="C2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="F20" s="34"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
         <v>110</v>
       </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" t="s">
         <v>108</v>
       </c>
-      <c r="C14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="37"/>
-      <c r="F20" s="36"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" t="s">
-        <v>113</v>
-      </c>
-      <c r="C27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="C29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="38" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="40" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -4155,17 +4108,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="90190796-45ad-4c96-92d3-17e9cee707e0">
-      <UserInfo>
-        <DisplayName>Vaccine Safety Members</DisplayName>
-        <AccountId>7</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4386,20 +4334,23 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="90190796-45ad-4c96-92d3-17e9cee707e0">
+      <UserInfo>
+        <DisplayName>Vaccine Safety Members</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EA9993F-454C-481A-9EAF-5876C98FD002}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171B7CA1-9B56-435E-B90C-D8382A40D1B3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="90190796-45ad-4c96-92d3-17e9cee707e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4424,9 +4375,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171B7CA1-9B56-435E-B90C-D8382A40D1B3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EA9993F-454C-481A-9EAF-5876C98FD002}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="90190796-45ad-4c96-92d3-17e9cee707e0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added back in protocol files, removed UCHEALTH for UCHDW
</commit_message>
<xml_diff>
--- a/extras/CovidAesiReporting/extras/Censorship Worksheet.xlsx
+++ b/extras/CovidAesiReporting/extras/Censorship Worksheet.xlsx
@@ -557,9 +557,6 @@
     <t>IMASIS</t>
   </si>
   <si>
-    <t>UCHEALTH</t>
-  </si>
-  <si>
     <t>CPRD_AURUM</t>
   </si>
   <si>
@@ -726,6 +723,9 @@
   </si>
   <si>
     <t>† COVID + Controls</t>
+  </si>
+  <si>
+    <t>UCHDW</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1095,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns="" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1618,8 +1618,8 @@
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="16" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>4</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="17" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>4</v>
@@ -2701,7 +2701,7 @@
     </row>
     <row r="18" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>61</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="19" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>4</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="20" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>4</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="21" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>61</v>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="22" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>61</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>4</v>
@@ -3103,7 +3103,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>4</v>
@@ -3170,23 +3170,23 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>85</v>
-      </c>
       <c r="G25" s="31" t="s">
         <v>4</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>4</v>
       </c>
       <c r="O25" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P25" s="31" t="s">
         <v>4</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>61</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="23" t="s">
         <v>4</v>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>61</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="23" t="s">
         <v>4</v>
@@ -3509,7 +3509,7 @@
     </row>
     <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>61</v>
@@ -3601,7 +3601,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="19" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="41"/>
     </row>
@@ -3615,10 +3615,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
         <v>92</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
       </c>
       <c r="C3">
         <v>71</v>
@@ -3641,10 +3641,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
         <v>94</v>
-      </c>
-      <c r="B4" t="s">
-        <v>95</v>
       </c>
       <c r="C4">
         <v>21</v>
@@ -3697,10 +3697,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5">
         <v>71</v>
@@ -3750,100 +3750,100 @@
   <sheetData>
     <row r="1" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="H1" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="I1" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="J1" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
         <v>107</v>
-      </c>
-      <c r="C2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
         <v>109</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
         <v>113</v>
       </c>
-      <c r="B6" t="s">
-        <v>114</v>
-      </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3851,10 +3851,10 @@
         <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3862,10 +3862,10 @@
         <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3873,10 +3873,10 @@
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3884,10 +3884,10 @@
         <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3895,10 +3895,10 @@
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3906,10 +3906,10 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3917,10 +3917,10 @@
         <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3928,21 +3928,21 @@
         <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3950,21 +3950,21 @@
         <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3972,21 +3972,21 @@
         <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D20" s="35"/>
       <c r="F20" s="34"/>
@@ -3996,10 +3996,10 @@
         <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4007,97 +4007,97 @@
         <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" t="s">
         <v>123</v>
       </c>
-      <c r="B25" t="s">
-        <v>124</v>
-      </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" t="s">
         <v>128</v>
       </c>
-      <c r="B29" t="s">
-        <v>129</v>
-      </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -4108,12 +4108,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="90190796-45ad-4c96-92d3-17e9cee707e0">
+      <UserInfo>
+        <DisplayName>Vaccine Safety Members</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4334,23 +4339,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="90190796-45ad-4c96-92d3-17e9cee707e0">
-      <UserInfo>
-        <DisplayName>Vaccine Safety Members</DisplayName>
-        <AccountId>7</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171B7CA1-9B56-435E-B90C-D8382A40D1B3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EA9993F-454C-481A-9EAF-5876C98FD002}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="90190796-45ad-4c96-92d3-17e9cee707e0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4375,11 +4377,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EA9993F-454C-481A-9EAF-5876C98FD002}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{171B7CA1-9B56-435E-B90C-D8382A40D1B3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="90190796-45ad-4c96-92d3-17e9cee707e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>